<commit_message>
Updated excel file for spike corr column definitions
</commit_message>
<xml_diff>
--- a/scripts/pairAnalysis/createDataset/spkCorrTableVariableDefs.xlsx
+++ b/scripts/pairAnalysis/createDataset/spkCorrTableVariableDefs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/subravcr/Projects/NEIWork/SATCorrelations/git/thomas-jpsth/scripts/pairAnalysis/createDataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74B7D42B-CB5B-4E4C-AAD7-0435AB733EA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E85834-B821-6141-99C6-6E7984C00BC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4820" yWindow="3540" windowWidth="38800" windowHeight="23940" xr2:uid="{1B6384B1-7DF6-F341-93CA-5C2CD1321281}"/>
   </bookViews>
@@ -336,6 +336,9 @@
     <t xml:space="preserve">'signifZTrial_01_200ms' </t>
   </si>
   <si>
+    <t xml:space="preserve">'xWaveMean' </t>
+  </si>
+  <si>
     <t>'xWaveStd'</t>
   </si>
   <si>
@@ -354,30 +357,6 @@
     <t>'yWaveWidthMean'</t>
   </si>
   <si>
-    <t xml:space="preserve">'yWaveWidthStd' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">'signifRaw_05_150ms: Is raw spike count correlation (rho)  in static 150 ms window significant at p &lt;= 0.05. Values 1 = significant &amp; 0 = not-significant.' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">'signifRaw_01_150ms: Is raw spike count correlation (rho)  in static 150 ms window significant at p &lt;= 0.01. Values 1 = significant &amp; 0 = not-significant.' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">'signifZBaseline_05_150ms: Is ZBaseline spike count correlation (rho)  in static 150 ms window significant at p &lt;= 0.05. Values 1 = significant &amp; 0 = not-significant.' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">'signifZBaseline_01_150ms: Is ZBaseline spike count correlation (rho)  in static 150 ms window significant at p &lt;= 0.01. Values 1 = significant &amp; 0 = not-significant.' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">'signifZTrial_05_150ms: Is ZTrial spike count correlation (rho)  in static 150 ms window significant at p &lt;= 0.05. Values 1 = significant &amp; 0 = not-significant.' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">'signifZTrial_01_150ms: Is ZTrial spike count correlation (rho)  in static 150 ms window significant at p &lt;= 0.01. Values 1 = significant &amp; 0 = not-significant.' </t>
-  </si>
-  <si>
-    <t>'srcFile: File containing spike count correlation (R_sc) as well as all other variables for this pair. This file is at spkCorr/spkCorr_[area1]-[area2]/mat/spkCorr_[Pair_UID].mat. Areas are [SEF | FEF | SC]. See pairAnalysis/createDataset/getSpkCorrForPair.m'</t>
-  </si>
-  <si>
     <t>'pairAreas: Areas of the two neurons included in this pair [SEF | FEF | SC].'</t>
   </si>
   <si>
@@ -396,12 +375,6 @@
     <t xml:space="preserve">'X_sess: Session ID for Neuron X of this pair.' </t>
   </si>
   <si>
-    <t>'X_unitNum: Unit number for Neuron X of this pair. The unitNum is the row num in table variables: unitInfo, unitStats in file dataset/dataNeurophys_SAT.mat '</t>
-  </si>
-  <si>
-    <t>'Y_unitNum: Unit number for Neuron Y of this pair. The unitNum is the row num in table variables: unitInfo, unitStats in file dataset/dataNeurophys_SAT.mat '</t>
-  </si>
-  <si>
     <t>'X_unit: Unit ID for Neuron X of this pair. These are char vectors corresponding to [channelNum][clusterId]. Eample 10a corresponding to DSP10a in the translated matlab datafile.'</t>
   </si>
   <si>
@@ -450,12 +423,6 @@
     <t xml:space="preserve">'Y_errGrade: Choice error-related activity grade for Neuron Y of this pair. Value range [-4 to +4]. Positive is error-enhanced. Negative is error-inhibited.' </t>
   </si>
   <si>
-    <t xml:space="preserve">'X_isErrGrade: Is Choice grade for Neuron X of this pair. Value range [0 | 1] . A Value of 1 = abs(X_errGrade)&gt;=2. ' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">'Y_isErrGrade: Is Choice grade for Neuron Y of this pair. Value range [0 | 1] . A Value of 1 = abs(Y_errGrade)&gt;=2. ' </t>
-  </si>
-  <si>
     <t>'X_errField: Choice error-related activity field for Neuron X of this pair. Value range [0 to 7]. Location of saccade for choice error trials.'</t>
   </si>
   <si>
@@ -468,12 +435,6 @@
     <t xml:space="preserve">'Y_rewGrade: Timing error-related activity grade for Neuron Y of this pair. Value range [-4 to +4]. Positive is error-enhanced. Negative is error-inhibited.' </t>
   </si>
   <si>
-    <t xml:space="preserve">'X_isRewGrade: Is timing error grade for Neuron X of this pair. Value range [0 | 1] . A Value of 1 = abs(X_rewGrade)&gt;=2. ' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">'Y_isRewGrade: Is timing error grade for Neuron Y of this pair. Value range [0 | 1] . A Value of 1 = abs(X_rewGrade)&gt;=2. ' </t>
-  </si>
-  <si>
     <t>'X_taskType: Level of search difficulty for Neuron X of this pair. Note: this is session-specific. 1=Easy &amp; 2=Hard.'</t>
   </si>
   <si>
@@ -483,18 +444,6 @@
     <t xml:space="preserve">'Y_Hemi: Hemifield for Neuron Y of this pair. Values [Left | Right]. These are copied from excel sheets in dataProcessed/excel folder.' </t>
   </si>
   <si>
-    <t>'X_Grid: Electrode grid location for Neuron X of this pair. Pair of values (in mm) that specify Anterior(a)/Posterior(p), Lateral(L)/Medial(M) of electrode. Example [4p,3L]'</t>
-  </si>
-  <si>
-    <t>'Y_Grid: Electrode grid location for Neuron Y of this pair. Pair of values (in mm) that specify Anterior(a)/Posterior(p), Lateral(L)/Medial(M) of electrode. Example [4p,3L]'</t>
-  </si>
-  <si>
-    <t>'X_Grid_AP_ML: Electrode grid location for Neuron X of this pair. Values are in +/- mm.  A sign of  positive = Anterior(a) for AP or Medial(M) for ML and a sign of negative = Posterior(p) for AP and Lateral(L) for ML.</t>
-  </si>
-  <si>
-    <t>'Y_Grid_AP_ML: Electrode grid location for Neuron Y of this pair. Values are in +/- mm.  A sign of  positive = Anterior(a) for AP or Medial(M) for ML and a sign of negative = Posterior(p) for AP and Lateral(L) for ML.</t>
-  </si>
-  <si>
     <t>'X_Depth: (From Rich) Observed recording depth in micrometers (um) for Neuron X of this pair. Not corrected for depth of dura or mis-alignment due to electrode lengths, etc. Very gross measure.'</t>
   </si>
   <si>
@@ -516,9 +465,6 @@
     <t>'XY_Depth: Euclidean distance (3-D) in mm, between recording contacts for Neuron X and Neuron Y of this pair.'</t>
   </si>
   <si>
-    <t>'isOnSameChannel: Neuron X and Neuron Y are from same channel. For example 13a and 13b. Ensure for this pair that the two neurons of the pair are distinct and not the same-neuron due to clustering issues in spike sorting.</t>
-  </si>
-  <si>
     <t xml:space="preserve">'condition: Is the trial outcome. This is a combination of SAT condition [Fast | Accurate] and trial outcome [Correct | ErrorChoice | ErrorTiming]. TODO: This field should be re-named (if renamed all code that refers to this have to change).' </t>
   </si>
   <si>
@@ -576,24 +522,6 @@
     <t>'rho_pval_static_Z_trial_200ms: Spike count correlation, after scaling each trial by mean and std of *trial* counts of all trials,  (rho) and pval computed for a 200ms static time window for this neuron pair for this condition and epoch combination. Example FastCorrect and Baseline. There are 6 conditions [Fast | Accurate] x [Correct | ErrorChoice | ErrorTiming] and 4 epochs [[Baseline | Visual | PostSaccade | PostReward].'</t>
   </si>
   <si>
-    <t xml:space="preserve">'signifRaw_05_50ms: Is raw spike count correlation (rho)  in static 50 ms window significant at p &lt;= 0.05. Values 1 = significant &amp; 0 = not-significant.' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">'signifRaw_01_50ms: Is raw spike count correlation (rho)  in static 50 ms window significant at p &lt;= 0.01. Values 1 = significant &amp; 0 = not-significant.' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">'signifZBaseline_05_50ms: Is ZBaseline spike count correlation (rho)  in static 50 ms window significant at p &lt;= 0.05. Values 1 = significant &amp; 0 = not-significant.' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">'signifZBaseline_01_50ms: Is ZBaseline spike count correlation (rho)  in static 50 ms window significant at p &lt;= 0.01. Values 1 = significant &amp; 0 = not-significant.' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">'signifZTrial_05_50ms: Is ZTrial spike count correlation (rho)  in static 50 ms window significant at p &lt;= 0.05. Values 1 = significant &amp; 0 = not-significant.' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">'signifZTrial_01_50ms: Is ZTrial spike count correlation (rho)  in static 50 ms window significant at p &lt;= 0.01. Values 1 = significant &amp; 0 = not-significant.' </t>
-  </si>
-  <si>
     <t xml:space="preserve">'rhoRaw_50ms: rho (r_sc spike count correlation) value from column rho_pval_static_50ms.' </t>
   </si>
   <si>
@@ -612,63 +540,24 @@
     <t xml:space="preserve">'pvalZTrial_50ms: pval value from column rho_pval_static_ZTrial_50ms.' </t>
   </si>
   <si>
-    <t xml:space="preserve">rhoRaw_150ms: rho (r_sc spike count correlation) value from column rho_pval_static_150ms.' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">pvalRaw_150ms: pval value from column rho_pval_static_150ms.' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rhoZBaseline_150ms: rho (r_sc spike count correlation) value from column rho_pval_static_Zbaseline_150ms.' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">pvalZBaseline_150ms: pval value from column rho_pval_static_Zbaseline_150ms.' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rhoZTrial_150ms: rho (r_sc spike count correlation) value from column rho_pval_static_ZTrial_150ms.' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">pvalZTrial_150ms: pval value from column rho_pval_static_ZTrial_150ms.' </t>
-  </si>
-  <si>
     <t xml:space="preserve">'rhoRaw_200ms: rho (r_sc spike count correlation) value from column rho_pval_static_200ms.' </t>
   </si>
   <si>
     <t xml:space="preserve">'pvalRaw_200ms: pval value from column rho_pval_static_200ms.' </t>
   </si>
   <si>
-    <t xml:space="preserve">'signifRaw_05_200ms: Is raw spike count correlation (rho)  in static 200 ms window significant at p &lt;= 0.05. Values 1 = significant &amp; 0 = not-significant.' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">'signifRaw_01_200ms: Is raw spike count correlation (rho)  in static 200 ms window significant at p &lt;= 0.01. Values 1 = significant &amp; 0 = not-significant.' </t>
-  </si>
-  <si>
     <t xml:space="preserve">'rhoZBaseline_200ms: rho (r_sc spike count correlation) value from column rho_pval_static_Zbaseline_200ms.' </t>
   </si>
   <si>
     <t xml:space="preserve">'pvalZBaseline_200ms: pval value from column rho_pval_static_Zbaseline_200ms.' </t>
   </si>
   <si>
-    <t xml:space="preserve">'signifZBaseline_05_200ms: Is ZBaseline spike count correlation (rho)  in static 200 ms window significant at p &lt;= 0.05. Values 1 = significant &amp; 0 = not-significant.' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">'signifZBaseline_01_200ms: Is ZBaseline spike count correlation (rho)  in static 200 ms window significant at p &lt;= 0.01. Values 1 = significant &amp; 0 = not-significant.' </t>
-  </si>
-  <si>
     <t xml:space="preserve">'rhoZTrial_200ms: rho (r_sc spike count correlation) value from column rho_pval_static_ZTrial_200ms.' </t>
   </si>
   <si>
     <t xml:space="preserve">'pvalZTrial_200ms: pval value from column rho_pval_static_ZTrial_200ms.' </t>
   </si>
   <si>
-    <t xml:space="preserve">'signifZTrial_05_200ms: Is ZTrial spike count correlation (rho)  in static 200 ms window significant at p &lt;= 0.05. Values 1 = significant &amp; 0 = not-significant.' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">'signifZTrial_01_200ms: Is ZTrial spike count correlation (rho)  in static 200 ms window significant at p &lt;= 0.01. Values 1 = significant &amp; 0 = not-significant.' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">xWaveMean' </t>
-  </si>
-  <si>
     <t xml:space="preserve">'xWaveMean: Mean waveform of Neuron X of this pair. Average of waveforms corresponding to all spikes for this condition and epoch.' </t>
   </si>
   <si>
@@ -690,7 +579,118 @@
     <t>'yWaveWidthMean: Mean waveform-width (in sampling ticks: 40KHz) of Neuron Y of this pair. For Waveforms corresponding to all spikes for this condition and epoch. Mean full-width between trough and peak of waveforms.'</t>
   </si>
   <si>
-    <t xml:space="preserve">'yWaveWidthStd: Stabdard deviation of waveform-widths (in sampling ticks: 40KHz) of Neuron Y of this pair. For Waveforms corresponding to all spikes for this condition and epoch. Stddev full-width between trough and peak of waveforms.' </t>
+    <t>'yWaveWidthStd'</t>
+  </si>
+  <si>
+    <t>'srcFile: File containing spike count correlation (R_sc) as well as all other variables for this pair. This file is at spkCorr/spkCorr_[area1]-[area2]/mat/spkCorr_[Pair_UID].mat. Areas are [SEF | FEF | SC]. See pairAnalysis/createDataset/getSpkCorrForPair.m.'</t>
+  </si>
+  <si>
+    <t>'X_unitNum: Unit number for Neuron X of this pair. The unitNum is the row num in table variables: unitInfo, unitStats in file dataset/dataNeurophys_SAT.mat.'</t>
+  </si>
+  <si>
+    <t>'Y_unitNum: Unit number for Neuron Y of this pair. The unitNum is the row num in table variables: unitInfo, unitStats in file dataset/dataNeurophys_SAT.mat.'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'X_isErrGrade: Is Choice grade for Neuron X of this pair. Value range [0 | 1] . A Value of 1 = abs(X_errGrade)&gt;=2.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'Y_isErrGrade: Is Choice grade for Neuron Y of this pair. Value range [0 | 1] . A Value of 1 = abs(Y_errGrade)&gt;=2.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'X_isRewGrade: Is timing error grade for Neuron X of this pair. Value range [0 | 1] . A Value of 1 = abs(X_rewGrade)&gt;=2.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'Y_isRewGrade: Is timing error grade for Neuron Y of this pair. Value range [0 | 1] . A Value of 1 = abs(X_rewGrade)&gt;=2.' </t>
+  </si>
+  <si>
+    <t>'X_Grid: Electrode grid location for Neuron X of this pair. Pair of values (in mm) that specify Anterior(a)/Posterior(p), Lateral(L)/Medial(M) of electrode. Example [4p,3L].'</t>
+  </si>
+  <si>
+    <t>'Y_Grid: Electrode grid location for Neuron Y of this pair. Pair of values (in mm) that specify Anterior(a)/Posterior(p), Lateral(L)/Medial(M) of electrode. Example [4p,3L].'</t>
+  </si>
+  <si>
+    <t>'X_Grid_AP_ML: Electrode grid location for Neuron X of this pair. Values are in +/- mm.  A sign of  positive = Anterior(a) for AP or Medial(M) for ML and a sign of negative = Posterior(p) for AP and Lateral(L) for ML.'</t>
+  </si>
+  <si>
+    <t>'Y_Grid_AP_ML: Electrode grid location for Neuron Y of this pair. Values are in +/- mm.  A sign of  positive = Anterior(a) for AP or Medial(M) for ML and a sign of negative = Posterior(p) for AP and Lateral(L) for ML.'</t>
+  </si>
+  <si>
+    <t>'isOnSameChannel: Neuron X and Neuron Y are from same channel. For example 13a and 13b. Ensure for this pair that the two neurons of the pair are distinct and not the same-neuron due to clustering issues in spike sorting.'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'signifRaw_05_50ms: Is raw spike count correlation (rho) in static 50 ms window significant at p &lt;= 0.05. Values 1 = significant &amp; 0 = not-significant.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'signifRaw_01_50ms: Is raw spike count correlation (rho) in static 50 ms window significant at p &lt;= 0.01. Values 1 = significant &amp; 0 = not-significant.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'signifZBaseline_05_50ms: Is ZBaseline spike count correlation (rho) in static 50 ms window significant at p &lt;= 0.05. Values 1 = significant &amp; 0 = not-significant.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'signifZBaseline_01_50ms: Is ZBaseline spike count correlation (rho) in static 50 ms window significant at p &lt;= 0.01. Values 1 = significant &amp; 0 = not-significant.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'signifZTrial_05_50ms: Is ZTrial spike count correlation (rho) in static 50 ms window significant at p &lt;= 0.05. Values 1 = significant &amp; 0 = not-significant.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'signifZTrial_01_50ms: Is ZTrial spike count correlation (rho) in static 50 ms window significant at p &lt;= 0.01. Values 1 = significant &amp; 0 = not-significant.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'rhoRaw_150ms: rho (r_sc spike count correlation) value from column rho_pval_static_150ms.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'pvalRaw_150ms: pval value from column rho_pval_static_150ms.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'signifRaw_05_150ms: Is raw spike count correlation (rho) in static 150 ms window significant at p &lt;= 0.05. Values 1 = significant &amp; 0 = not-significant.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'signifRaw_01_150ms: Is raw spike count correlation (rho) in static 150 ms window significant at p &lt;= 0.01. Values 1 = significant &amp; 0 = not-significant.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'rhoZBaseline_150ms: rho (r_sc spike count correlation) value from column rho_pval_static_Zbaseline_150ms.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'pvalZBaseline_150ms: pval value from column rho_pval_static_Zbaseline_150ms.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'signifZBaseline_05_150ms: Is ZBaseline spike count correlation (rho) in static 150 ms window significant at p &lt;= 0.05. Values 1 = significant &amp; 0 = not-significant.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'signifZBaseline_01_150ms: Is ZBaseline spike count correlation (rho) in static 150 ms window significant at p &lt;= 0.01. Values 1 = significant &amp; 0 = not-significant.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'rhoZTrial_150ms: rho (r_sc spike count correlation) value from column rho_pval_static_ZTrial_150ms.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'pvalZTrial_150ms: pval value from column rho_pval_static_ZTrial_150ms.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'signifZTrial_05_150ms: Is ZTrial spike count correlation (rho) in static 150 ms window significant at p &lt;= 0.05. Values 1 = significant &amp; 0 = not-significant.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'signifZTrial_01_150ms: Is ZTrial spike count correlation (rho) in static 150 ms window significant at p &lt;= 0.01. Values 1 = significant &amp; 0 = not-significant.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'signifRaw_05_200ms: Is raw spike count correlation (rho) in static 200 ms window significant at p &lt;= 0.05. Values 1 = significant &amp; 0 = not-significant.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'signifRaw_01_200ms: Is raw spike count correlation (rho) in static 200 ms window significant at p &lt;= 0.01. Values 1 = significant &amp; 0 = not-significant.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'signifZBaseline_05_200ms: Is ZBaseline spike count correlation (rho) in static 200 ms window significant at p &lt;= 0.05. Values 1 = significant &amp; 0 = not-significant.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'signifZBaseline_01_200ms: Is ZBaseline spike count correlation (rho) in static 200 ms window significant at p &lt;= 0.01. Values 1 = significant &amp; 0 = not-significant.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'signifZTrial_05_200ms: Is ZTrial spike count correlation (rho) in static 200 ms window significant at p &lt;= 0.05. Values 1 = significant &amp; 0 = not-significant.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'signifZTrial_01_200ms: Is ZTrial spike count correlation (rho) in static 200 ms window significant at p &lt;= 0.01. Values 1 = significant &amp; 0 = not-significant.' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">yWaveWidthStd: Standard deviation of waveform-widths (in sampling ticks: 40KHz) of Neuron Y of this pair. For Waveforms corresponding to all spikes for this condition and epoch. Stddev full-width between trough and peak of waveforms.'  </t>
   </si>
 </sst>
 </file>
@@ -1053,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0457EA2C-BDE2-5149-9F10-F04303309F8C}">
   <dimension ref="A1:B111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B118" sqref="B118"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1068,7 +1068,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>116</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1076,7 +1076,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1084,7 +1084,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1092,7 +1092,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1100,7 +1100,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1108,7 +1108,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1116,7 +1116,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1124,7 +1124,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>123</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1132,7 +1132,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>124</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1140,7 +1140,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1148,7 +1148,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1156,7 +1156,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1164,7 +1164,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1172,7 +1172,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1180,7 +1180,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -1188,7 +1188,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1196,7 +1196,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -1204,7 +1204,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1212,7 +1212,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1220,7 +1220,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1228,7 +1228,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -1236,7 +1236,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -1244,7 +1244,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -1252,7 +1252,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -1260,7 +1260,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -1268,7 +1268,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>141</v>
+        <v>188</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -1276,7 +1276,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>142</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -1284,7 +1284,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -1292,7 +1292,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1300,7 +1300,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -1308,7 +1308,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -1316,7 +1316,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>147</v>
+        <v>190</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -1324,7 +1324,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>148</v>
+        <v>191</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -1332,7 +1332,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -1340,7 +1340,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -1348,7 +1348,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -1356,7 +1356,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>152</v>
+        <v>192</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -1364,7 +1364,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>153</v>
+        <v>193</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -1372,7 +1372,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>154</v>
+        <v>194</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -1380,7 +1380,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>155</v>
+        <v>195</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -1388,7 +1388,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -1396,7 +1396,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -1404,7 +1404,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -1412,7 +1412,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -1420,7 +1420,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -1428,7 +1428,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -1436,7 +1436,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -1444,7 +1444,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>163</v>
+        <v>196</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -1452,7 +1452,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -1460,7 +1460,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -1468,7 +1468,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -1476,7 +1476,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -1484,7 +1484,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -1492,7 +1492,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -1500,7 +1500,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -1508,7 +1508,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -1516,7 +1516,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -1524,7 +1524,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -1532,7 +1532,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -1540,7 +1540,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -1548,7 +1548,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -1556,7 +1556,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -1564,7 +1564,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -1572,7 +1572,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -1580,7 +1580,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -1588,7 +1588,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -1596,7 +1596,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
@@ -1604,7 +1604,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
@@ -1612,7 +1612,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
@@ -1620,7 +1620,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
@@ -1628,7 +1628,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
@@ -1636,7 +1636,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
@@ -1644,7 +1644,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
@@ -1652,7 +1652,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
@@ -1660,7 +1660,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
@@ -1668,7 +1668,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
@@ -1676,7 +1676,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
@@ -1684,7 +1684,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
@@ -1692,7 +1692,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
@@ -1700,7 +1700,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
@@ -1708,7 +1708,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
@@ -1716,7 +1716,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>110</v>
+        <v>205</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
@@ -1724,7 +1724,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>111</v>
+        <v>206</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
@@ -1732,7 +1732,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
@@ -1740,7 +1740,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
@@ -1748,7 +1748,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>112</v>
+        <v>209</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
@@ -1756,7 +1756,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>113</v>
+        <v>210</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
@@ -1764,7 +1764,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
@@ -1772,7 +1772,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
@@ -1780,7 +1780,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>114</v>
+        <v>213</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
@@ -1788,7 +1788,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>115</v>
+        <v>214</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
@@ -1796,7 +1796,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>201</v>
+        <v>171</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
@@ -1804,7 +1804,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>202</v>
+        <v>172</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
@@ -1812,7 +1812,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
@@ -1820,7 +1820,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
@@ -1828,7 +1828,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>205</v>
+        <v>173</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
@@ -1836,7 +1836,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>206</v>
+        <v>174</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
@@ -1844,7 +1844,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
@@ -1852,7 +1852,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
@@ -1860,7 +1860,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>209</v>
+        <v>175</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
@@ -1868,7 +1868,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>210</v>
+        <v>176</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
@@ -1876,7 +1876,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
@@ -1884,70 +1884,70 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>213</v>
+        <v>103</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>214</v>
+        <v>177</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>215</v>
+        <v>178</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>216</v>
+        <v>179</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>217</v>
+        <v>180</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>218</v>
+        <v>181</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>219</v>
+        <v>182</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>220</v>
+        <v>183</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>109</v>
-      </c>
-      <c r="B111" t="s">
+        <v>184</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>221</v>
       </c>
     </row>

</xml_diff>